<commit_message>
Actualizações ao diagrama de classes e casos de uso
Trabalhamos 45 minutos no total
Luis Soares e João Freire
</commit_message>
<xml_diff>
--- a/Engenharia de Software/descricao de caso de uso.xlsx
+++ b/Engenharia de Software/descricao de caso de uso.xlsx
@@ -5,16 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis_\Documents\GitHub\Engenharia-software-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis_\Documents\GitHub\EngSof2-ProgInter\Engenharia de Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Escolher inquerito" sheetId="1" r:id="rId1"/>
     <sheet name="Criar Trilho" sheetId="2" r:id="rId2"/>
     <sheet name="Alterar trilho" sheetId="3" r:id="rId3"/>
+    <sheet name="Alterar inquérito" sheetId="4" r:id="rId4"/>
+    <sheet name="Consultar inquérito" sheetId="5" r:id="rId5"/>
+    <sheet name="Eliminar inquérito" sheetId="6" r:id="rId6"/>
+    <sheet name="Criar Utente" sheetId="7" r:id="rId7"/>
+    <sheet name="Consultar Utente" sheetId="8" r:id="rId8"/>
+    <sheet name="Alterar Utente" sheetId="9" r:id="rId9"/>
+    <sheet name="Eliminar Utente" sheetId="10" r:id="rId10"/>
+    <sheet name="Criar questionario" sheetId="11" r:id="rId11"/>
+    <sheet name="Alterar questionario" sheetId="12" r:id="rId12"/>
+    <sheet name="eliminar questionario" sheetId="13" r:id="rId13"/>
+    <sheet name="consultar questionario" sheetId="14" r:id="rId14"/>
+    <sheet name="Comparar trilhos" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="76">
   <si>
     <t>nome</t>
   </si>
@@ -185,6 +197,75 @@
   </si>
   <si>
     <t>o sistema devolve uma mensagem de erro na alteração de dados</t>
+  </si>
+  <si>
+    <t>Criar utente</t>
+  </si>
+  <si>
+    <t>o ator vai criar o seu profile</t>
+  </si>
+  <si>
+    <t>clicar no botão registar</t>
+  </si>
+  <si>
+    <t>o sistema devolve uma lista com todos os dados a preencher</t>
+  </si>
+  <si>
+    <t>o sistema devolve uma mensagem de sucesso</t>
+  </si>
+  <si>
+    <t>o ator clica no botão registar</t>
+  </si>
+  <si>
+    <t>Já existe alguem registado</t>
+  </si>
+  <si>
+    <t>verificar se o sistema devolve os dados necessarios</t>
+  </si>
+  <si>
+    <t>Consultar utente</t>
+  </si>
+  <si>
+    <t>o ator vai consultar o seu profile</t>
+  </si>
+  <si>
+    <t>clicar no botão profile</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario com o profile do utente</t>
+  </si>
+  <si>
+    <t>login feito</t>
+  </si>
+  <si>
+    <t>Alterar utente</t>
+  </si>
+  <si>
+    <t>o ator vai alterar o seu profile</t>
+  </si>
+  <si>
+    <t>o ator clicar no botão profile</t>
+  </si>
+  <si>
+    <t>o ator clica no botão alterar</t>
+  </si>
+  <si>
+    <t>o ator altera os dados pretendidos e clica no botao alterar</t>
+  </si>
+  <si>
+    <t>Eliminar utente</t>
+  </si>
+  <si>
+    <t>o ator vai Eliminar o seu profile</t>
+  </si>
+  <si>
+    <t>o ator clica no botão eliminar</t>
+  </si>
+  <si>
+    <t>o sistema devolve uma mensagem a solicitar confirmação</t>
+  </si>
+  <si>
+    <t>o ator confirma</t>
   </si>
 </sst>
 </file>
@@ -654,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,11 +922,249 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1219,4 +1538,552 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
actualizações gerais a engenharia de software
</commit_message>
<xml_diff>
--- a/Engenharia de Software/descricao de caso de uso.xlsx
+++ b/Engenharia de Software/descricao de caso de uso.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Escolher inquerito" sheetId="1" r:id="rId1"/>
-    <sheet name="Criar Trilho" sheetId="2" r:id="rId2"/>
-    <sheet name="Alterar trilho" sheetId="3" r:id="rId3"/>
+    <sheet name="Criar Trilho" sheetId="2" r:id="rId1"/>
+    <sheet name="Alterar trilho" sheetId="3" r:id="rId2"/>
+    <sheet name="Criar inquerito" sheetId="16" r:id="rId3"/>
     <sheet name="Alterar inquérito" sheetId="4" r:id="rId4"/>
     <sheet name="Consultar inquérito" sheetId="5" r:id="rId5"/>
     <sheet name="Eliminar inquérito" sheetId="6" r:id="rId6"/>
@@ -22,11 +22,12 @@
     <sheet name="Consultar Utente" sheetId="8" r:id="rId8"/>
     <sheet name="Alterar Utente" sheetId="9" r:id="rId9"/>
     <sheet name="Eliminar Utente" sheetId="10" r:id="rId10"/>
-    <sheet name="Criar questionario" sheetId="11" r:id="rId11"/>
+    <sheet name="Responder questionario" sheetId="11" r:id="rId11"/>
     <sheet name="Alterar questionario" sheetId="12" r:id="rId12"/>
     <sheet name="eliminar questionario" sheetId="13" r:id="rId13"/>
     <sheet name="consultar questionario" sheetId="14" r:id="rId14"/>
     <sheet name="Comparar trilhos" sheetId="15" r:id="rId15"/>
+    <sheet name="Escolher inquerito" sheetId="1" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="87">
   <si>
     <t>nome</t>
   </si>
@@ -266,6 +267,39 @@
   </si>
   <si>
     <t>o ator confirma</t>
+  </si>
+  <si>
+    <t>Responder questionario</t>
+  </si>
+  <si>
+    <t>o ator vai responder ao questionario</t>
+  </si>
+  <si>
+    <t>clicar no botão questionario</t>
+  </si>
+  <si>
+    <t>login, inqueritos</t>
+  </si>
+  <si>
+    <t>o sistema devolve um questionario</t>
+  </si>
+  <si>
+    <t>o ator responde ao questionario e clica em submeter</t>
+  </si>
+  <si>
+    <t>O sistema não devolve um questionario</t>
+  </si>
+  <si>
+    <t>Criar Inquérito</t>
+  </si>
+  <si>
+    <t>o ator vai criar o inquerito</t>
+  </si>
+  <si>
+    <t>clicar no botão novo</t>
+  </si>
+  <si>
+    <t>o ator preenche os dados e clica em submeter</t>
   </si>
 </sst>
 </file>
@@ -735,21 +769,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -760,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -776,7 +806,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +820,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -806,7 +836,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,7 +844,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -832,20 +862,24 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -882,7 +916,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -890,7 +924,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -898,7 +932,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -918,7 +952,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -927,7 +960,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,12 +1135,174 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1160,21 +1355,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1185,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1193,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1201,7 +1400,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1215,7 +1414,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1223,7 +1422,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1231,7 +1430,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1239,7 +1438,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1257,24 +1456,20 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1311,7 +1506,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1319,7 +1514,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1327,7 +1522,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1347,10 +1542,11 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -1519,6 +1715,174 @@
       <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>

</xml_diff>

<commit_message>
Correção de alguns erros
Luis Soares e Joao Freire
</commit_message>
<xml_diff>
--- a/Engenharia de Software/descricao de caso de uso.xlsx
+++ b/Engenharia de Software/descricao de caso de uso.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" firstSheet="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Criar inquerito" sheetId="16" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <sheet name="Escolher inquerito" sheetId="1" r:id="rId12"/>
     <sheet name="Criar Trilho" sheetId="2" r:id="rId13"/>
     <sheet name="Alterar trilho" sheetId="3" r:id="rId14"/>
-    <sheet name="Comparar trilhos" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -840,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B18"/>
     </sheetView>
   </sheetViews>
@@ -1689,7 +1688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1871,18 +1870,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>